<commit_message>
Fixed Database columns to Kenia's format
</commit_message>
<xml_diff>
--- a/Scripts/data/data.xlsx
+++ b/Scripts/data/data.xlsx
@@ -13,12 +13,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="140">
   <si>
     <t>Nombre del proyecto-equipo</t>
   </si>
   <si>
-    <t>Categoria (debe ser igual que en la 3ra pestaña de este documento)</t>
+    <t>Categoria (debe ser IDENTICO que en la 3ra pestaña de este documento)</t>
+  </si>
+  <si>
+    <t>Modalidad (Demostración, Poster o Competencia)</t>
   </si>
   <si>
     <t>Nombres de integrantes sepadados por comas</t>
@@ -42,6 +45,9 @@
     <t>IA</t>
   </si>
   <si>
+    <t>Demostración</t>
+  </si>
+  <si>
     <t>Daniel Cruz, David Roldan</t>
   </si>
   <si>
@@ -54,7 +60,7 @@
     <t>Este proyecto está chido</t>
   </si>
   <si>
-    <t>Paralelo, Admin, Calidad de software</t>
+    <t>Paralelo, testing</t>
   </si>
   <si>
     <t>Equipo explosion</t>
@@ -63,6 +69,9 @@
     <t>Software</t>
   </si>
   <si>
+    <t>Poster</t>
+  </si>
+  <si>
     <t>Michelle Muñiz, Gustavo Algo</t>
   </si>
   <si>
@@ -75,7 +84,307 @@
     <t>Este proyecto está bonito</t>
   </si>
   <si>
-    <t>Front-End</t>
+    <t>Front-End, base de datos</t>
+  </si>
+  <si>
+    <t>equiplo delta</t>
+  </si>
+  <si>
+    <t>juan sachez, miguel</t>
+  </si>
+  <si>
+    <t>t01213,t03421</t>
+  </si>
+  <si>
+    <t>Este proyecto está nuevo</t>
+  </si>
+  <si>
+    <t>prototipos, UI/UX</t>
+  </si>
+  <si>
+    <t>equipo alpha</t>
+  </si>
+  <si>
+    <t>electronica</t>
+  </si>
+  <si>
+    <t>carlos, mateo</t>
+  </si>
+  <si>
+    <t>t00234,t23456</t>
+  </si>
+  <si>
+    <t>ICM,ICE</t>
+  </si>
+  <si>
+    <t>admin, testing</t>
+  </si>
+  <si>
+    <t>equipo tango</t>
+  </si>
+  <si>
+    <t>marco, esteban</t>
+  </si>
+  <si>
+    <t>t97544,t12353</t>
+  </si>
+  <si>
+    <t>ICM,ICC</t>
+  </si>
+  <si>
+    <t>GPU, paralelo</t>
+  </si>
+  <si>
+    <t>equipo foxtrot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isabella , alex </t>
+  </si>
+  <si>
+    <t>t46585,t98456</t>
+  </si>
+  <si>
+    <t>ICE,ICE</t>
+  </si>
+  <si>
+    <t>Este proyecto está aburrido</t>
+  </si>
+  <si>
+    <t>sensores,paralelo</t>
+  </si>
+  <si>
+    <t>equipo x-ray</t>
+  </si>
+  <si>
+    <t>compiladores</t>
+  </si>
+  <si>
+    <t>Competencia</t>
+  </si>
+  <si>
+    <t>alejandro, juan lopez</t>
+  </si>
+  <si>
+    <t>t21236,t32489</t>
+  </si>
+  <si>
+    <t>ICC,ICM</t>
+  </si>
+  <si>
+    <t>calidad de software,sensores</t>
+  </si>
+  <si>
+    <t>equipo mike</t>
+  </si>
+  <si>
+    <t>lucas, valentina</t>
+  </si>
+  <si>
+    <t>t02321,t43247</t>
+  </si>
+  <si>
+    <t>IER,ICC</t>
+  </si>
+  <si>
+    <t>equpo lima-limon</t>
+  </si>
+  <si>
+    <t>software</t>
+  </si>
+  <si>
+    <t>sofia,camila</t>
+  </si>
+  <si>
+    <t>t90604,t08662</t>
+  </si>
+  <si>
+    <t>Este proyecto está complejo</t>
+  </si>
+  <si>
+    <t>mecatronica</t>
+  </si>
+  <si>
+    <t>equipo omega</t>
+  </si>
+  <si>
+    <t>miguel, daniel rojas</t>
+  </si>
+  <si>
+    <t>t55345,t88088</t>
+  </si>
+  <si>
+    <t>IER,ICM</t>
+  </si>
+  <si>
+    <t>aerodimanica</t>
+  </si>
+  <si>
+    <t>equipo gamma</t>
+  </si>
+  <si>
+    <t>juan plablo, alexander</t>
+  </si>
+  <si>
+    <t>t84623,t86444</t>
+  </si>
+  <si>
+    <t>ICC, ICC</t>
+  </si>
+  <si>
+    <t>Este proyecto está avanzado</t>
+  </si>
+  <si>
+    <t>equipo taco-man</t>
+  </si>
+  <si>
+    <t>samuel, angelica</t>
+  </si>
+  <si>
+    <t>t84999,t93268</t>
+  </si>
+  <si>
+    <t>Este proyecto está dificil</t>
+  </si>
+  <si>
+    <t>front-end</t>
+  </si>
+  <si>
+    <t>equipo maravilla</t>
+  </si>
+  <si>
+    <t>ana martines, maria</t>
+  </si>
+  <si>
+    <t>t00324,t00341</t>
+  </si>
+  <si>
+    <t>Este proyecto esta tanquilo</t>
+  </si>
+  <si>
+    <t>UI/UX</t>
+  </si>
+  <si>
+    <t>equipo pi</t>
+  </si>
+  <si>
+    <t>robotica</t>
+  </si>
+  <si>
+    <t>alejandra, samanta</t>
+  </si>
+  <si>
+    <t>t03452,t46257</t>
+  </si>
+  <si>
+    <t>ICR,ICR</t>
+  </si>
+  <si>
+    <t>prototipos</t>
+  </si>
+  <si>
+    <t>equipo equix</t>
+  </si>
+  <si>
+    <t>pepe,felipe</t>
+  </si>
+  <si>
+    <t>t00023,t03346</t>
+  </si>
+  <si>
+    <t>equipo hills</t>
+  </si>
+  <si>
+    <t>antonio, carlos</t>
+  </si>
+  <si>
+    <t>t04321,t66422</t>
+  </si>
+  <si>
+    <t>ICC,ICR</t>
+  </si>
+  <si>
+    <t>equipo filiphs</t>
+  </si>
+  <si>
+    <t>alexander, ximmena</t>
+  </si>
+  <si>
+    <t>t88565,23579</t>
+  </si>
+  <si>
+    <t>IER,ICR</t>
+  </si>
+  <si>
+    <t>equipo sirend</t>
+  </si>
+  <si>
+    <t>melina, jorge g</t>
+  </si>
+  <si>
+    <t>t32771,t32811</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>equpo gapee</t>
+  </si>
+  <si>
+    <t>angel, erick</t>
+  </si>
+  <si>
+    <t>t19996,56455</t>
+  </si>
+  <si>
+    <t>ICM,ICM</t>
+  </si>
+  <si>
+    <t>equipo epsilon</t>
+  </si>
+  <si>
+    <t>gustavo A, gerardo</t>
+  </si>
+  <si>
+    <t>t77777,t11111</t>
+  </si>
+  <si>
+    <t>ICR,IER</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>equipo kartarios</t>
+  </si>
+  <si>
+    <t>sanchez, marco</t>
+  </si>
+  <si>
+    <t>t76113,t12137</t>
+  </si>
+  <si>
+    <t>Este proyecto esta completo</t>
+  </si>
+  <si>
+    <t>equipo noviembre</t>
+  </si>
+  <si>
+    <t>jorge, juan 2</t>
+  </si>
+  <si>
+    <t>t42342,t67244</t>
+  </si>
+  <si>
+    <t>IER,IER</t>
+  </si>
+  <si>
+    <t>equipo octubre</t>
+  </si>
+  <si>
+    <t>daniel 2, jose angel</t>
+  </si>
+  <si>
+    <t>t39394,t99993</t>
   </si>
   <si>
     <t>correo del evaluador</t>
@@ -96,10 +405,31 @@
     <t>IA, Software</t>
   </si>
   <si>
-    <t>kenia.os@cetys.mx</t>
-  </si>
-  <si>
-    <t>Kenia Os</t>
+    <t>kenia.picos@cetys.mx</t>
+  </si>
+  <si>
+    <t>Kenia Picos</t>
+  </si>
+  <si>
+    <t>enrique.montoya@cetys</t>
+  </si>
+  <si>
+    <t>enrique montoya</t>
+  </si>
+  <si>
+    <t>eletronica</t>
+  </si>
+  <si>
+    <t>david.domingo@cetys</t>
+  </si>
+  <si>
+    <t>david domingo</t>
+  </si>
+  <si>
+    <t>jean.paul@cetys</t>
+  </si>
+  <si>
+    <t>jean paul</t>
   </si>
   <si>
     <t>Nombre de las categorias</t>
@@ -142,17 +472,26 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -381,10 +720,10 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="26.75"/>
     <col customWidth="1" min="2" max="2" width="31.75"/>
-    <col customWidth="1" min="3" max="3" width="18.75"/>
-    <col customWidth="1" min="4" max="4" width="38.88"/>
-    <col customWidth="1" min="5" max="5" width="28.5"/>
-    <col customWidth="1" min="6" max="6" width="21.88"/>
+    <col customWidth="1" min="3" max="4" width="18.75"/>
+    <col customWidth="1" min="5" max="5" width="38.88"/>
+    <col customWidth="1" min="6" max="6" width="28.5"/>
+    <col customWidth="1" min="7" max="7" width="21.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -394,13 +733,13 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -409,51 +748,606 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>20</v>
+      <c r="D4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -477,36 +1371,69 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>23</v>
+      <c r="A1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>26</v>
+      <c r="A2" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
+      <c r="A3" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -528,18 +1455,33 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>29</v>
+      <c r="A1" s="6" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
+      <c r="A2" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>15</v>
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>